<commit_message>
remove alias column from urban_ath trimester xlsx
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_0/1_0_trimester_rep.xlsx
+++ b/dictionaries/urban_ath/1_0/1_0_trimester_rep.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" state="visible" r:id="rId2"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="303">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alias</t>
   </si>
   <si>
     <t xml:space="preserve">row_id</t>
@@ -1565,13 +1562,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C101" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="26"/>
@@ -1590,1386 +1587,1383 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="0" t="s">
+      <c r="D14" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>51</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>55</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="0" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C31" s="0" t="s">
+      <c r="D31" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="0" t="s">
+      <c r="D33" s="0" t="s">
         <v>77</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="D35" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C37" s="0" t="s">
+      <c r="D37" s="0" t="s">
         <v>87</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="0" t="s">
         <v>93</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C43" s="0" t="s">
+      <c r="D43" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="D43" s="0" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="0" t="s">
         <v>102</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C46" s="0" t="s">
+      <c r="D46" s="0" t="s">
         <v>107</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C47" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="0" t="s">
+      <c r="D47" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C49" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="0" t="s">
+      <c r="D49" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D50" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C51" s="0" t="s">
+      <c r="D51" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D53" s="0" t="s">
         <v>124</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="B54" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" s="0" t="s">
         <v>128</v>
-      </c>
-      <c r="B55" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" s="0" t="s">
         <v>130</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" s="0" t="s">
         <v>132</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C57" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="0" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="0" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="0" t="s">
         <v>136</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="0" t="s">
         <v>140</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D62" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="B62" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D63" s="0" t="s">
         <v>144</v>
-      </c>
-      <c r="B63" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D64" s="0" t="s">
         <v>146</v>
-      </c>
-      <c r="B64" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C64" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D64" s="0" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D65" s="0" t="s">
         <v>148</v>
-      </c>
-      <c r="B65" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D66" s="0" t="s">
         <v>150</v>
-      </c>
-      <c r="B66" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D67" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="B67" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D68" s="0" t="s">
         <v>154</v>
-      </c>
-      <c r="B68" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D69" s="0" t="s">
         <v>156</v>
-      </c>
-      <c r="B69" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D70" s="0" t="s">
         <v>158</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="0" t="s">
         <v>160</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D71" s="0" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D72" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C72" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D72" s="0" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="0" t="s">
         <v>164</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D73" s="0" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="0" t="s">
         <v>166</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D74" s="0" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="B75" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C75" s="0" t="s">
+      <c r="D75" s="0" t="s">
         <v>169</v>
-      </c>
-      <c r="D75" s="0" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="B76" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C76" s="0" t="s">
+      <c r="D76" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="D76" s="0" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="D77" s="0" t="s">
         <v>174</v>
-      </c>
-      <c r="B77" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C77" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="D77" s="0" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B78" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C78" s="0" t="s">
+      <c r="D78" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="D78" s="0" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B79" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C79" s="0" t="s">
+      <c r="D79" s="0" t="s">
         <v>180</v>
-      </c>
-      <c r="D79" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="D80" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C80" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="D80" s="0" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="0" t="s">
         <v>184</v>
-      </c>
-      <c r="B81" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D81" s="0" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="0" t="s">
         <v>186</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D82" s="0" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D83" s="0" t="s">
         <v>188</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C83" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D83" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D84" s="0" t="s">
         <v>190</v>
-      </c>
-      <c r="B84" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C84" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="D84" s="0" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C85" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B85" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" s="0" t="s">
+      <c r="D85" s="0" t="s">
         <v>193</v>
-      </c>
-      <c r="D85" s="0" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D86" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C86" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D86" s="0" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="B87" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D87" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="B87" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C87" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D87" s="0" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D88" s="0" t="s">
         <v>199</v>
-      </c>
-      <c r="B88" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D88" s="0" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="0" t="s">
         <v>201</v>
-      </c>
-      <c r="B89" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D89" s="0" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D90" s="0" t="s">
         <v>203</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D90" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="B91" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D91" s="0" t="s">
         <v>205</v>
-      </c>
-      <c r="B91" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C91" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D91" s="0" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B92" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D92" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="B92" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C92" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D92" s="0" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="B93" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D93" s="0" t="s">
         <v>209</v>
-      </c>
-      <c r="B93" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C93" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D93" s="0" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D94" s="0" t="s">
         <v>211</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="D94" s="0" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C95" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B95" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" s="0" t="s">
+      <c r="D95" s="0" t="s">
         <v>214</v>
-      </c>
-      <c r="D95" s="0" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C96" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B96" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" s="0" t="s">
+      <c r="D96" s="0" t="s">
         <v>217</v>
-      </c>
-      <c r="D96" s="0" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B97" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C97" s="0" t="s">
+      <c r="D97" s="0" t="s">
         <v>220</v>
-      </c>
-      <c r="D97" s="0" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C98" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B98" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C98" s="0" t="s">
+      <c r="D98" s="0" t="s">
         <v>223</v>
-      </c>
-      <c r="D98" s="0" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D99" s="0" t="s">
         <v>225</v>
-      </c>
-      <c r="B99" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C99" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="D99" s="0" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
+        <v>226</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>222</v>
+      </c>
+      <c r="D100" s="0" t="s">
         <v>227</v>
-      </c>
-      <c r="B100" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C100" s="0" t="s">
-        <v>223</v>
-      </c>
-      <c r="D100" s="0" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="D101" s="0" t="s">
         <v>229</v>
-      </c>
-      <c r="B101" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="D101" s="0" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
+        <v>230</v>
+      </c>
+      <c r="B102" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="D102" s="0" t="s">
         <v>231</v>
-      </c>
-      <c r="B102" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C102" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D102" s="0" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2991,11 +2985,11 @@
   </sheetPr>
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="1:1048576"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26"/>
@@ -3003,13 +2997,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>233</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>234</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>3</v>
@@ -3017,7 +3011,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>101</v>
@@ -3027,12 +3021,12 @@
         <v>0</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>102</v>
@@ -3042,12 +3036,12 @@
         <v>0</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>103</v>
@@ -3057,12 +3051,12 @@
         <v>0</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>104</v>
@@ -3072,12 +3066,12 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>105</v>
@@ -3087,12 +3081,12 @@
         <v>0</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>106</v>
@@ -3102,12 +3096,12 @@
         <v>0</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>107</v>
@@ -3117,12 +3111,12 @@
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>108</v>
@@ -3132,12 +3126,12 @@
         <v>0</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>109</v>
@@ -3147,12 +3141,12 @@
         <v>0</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>110</v>
@@ -3162,12 +3156,12 @@
         <v>0</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>111</v>
@@ -3177,12 +3171,12 @@
         <v>0</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>112</v>
@@ -3192,12 +3186,12 @@
         <v>0</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>113</v>
@@ -3207,12 +3201,12 @@
         <v>0</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>114</v>
@@ -3222,12 +3216,12 @@
         <v>0</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>115</v>
@@ -3237,12 +3231,12 @@
         <v>0</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>116</v>
@@ -3252,12 +3246,12 @@
         <v>0</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>117</v>
@@ -3267,12 +3261,12 @@
         <v>0</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>118</v>
@@ -3282,12 +3276,12 @@
         <v>0</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>119</v>
@@ -3297,12 +3291,12 @@
         <v>0</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>120</v>
@@ -3312,12 +3306,12 @@
         <v>0</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>121</v>
@@ -3327,12 +3321,12 @@
         <v>0</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>122</v>
@@ -3342,12 +3336,12 @@
         <v>0</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>123</v>
@@ -3357,12 +3351,12 @@
         <v>0</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>124</v>
@@ -3372,12 +3366,12 @@
         <v>0</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>125</v>
@@ -3387,12 +3381,12 @@
         <v>0</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>126</v>
@@ -3402,12 +3396,12 @@
         <v>0</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>127</v>
@@ -3417,12 +3411,12 @@
         <v>0</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>128</v>
@@ -3432,12 +3426,12 @@
         <v>0</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>129</v>
@@ -3447,12 +3441,12 @@
         <v>0</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>130</v>
@@ -3462,12 +3456,12 @@
         <v>0</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>131</v>
@@ -3477,12 +3471,12 @@
         <v>0</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>1001</v>
@@ -3492,12 +3486,12 @@
         <v>0</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>1102</v>
@@ -3507,12 +3501,12 @@
         <v>0</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>1103</v>
@@ -3522,12 +3516,12 @@
         <v>0</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>1104</v>
@@ -3537,12 +3531,12 @@
         <v>0</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>1201</v>
@@ -3552,12 +3546,12 @@
         <v>0</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>1202</v>
@@ -3567,12 +3561,12 @@
         <v>0</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>1203</v>
@@ -3582,12 +3576,12 @@
         <v>0</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>1204</v>
@@ -3597,12 +3591,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>1205</v>
@@ -3612,12 +3606,12 @@
         <v>0</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>1301</v>
@@ -3627,12 +3621,12 @@
         <v>0</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>1401</v>
@@ -3642,12 +3636,12 @@
         <v>0</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>1402</v>
@@ -3657,12 +3651,12 @@
         <v>0</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>1403</v>
@@ -3672,12 +3666,12 @@
         <v>0</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>1404</v>
@@ -3687,12 +3681,12 @@
         <v>0</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>1501</v>
@@ -3702,12 +3696,12 @@
         <v>0</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>1601</v>
@@ -3717,12 +3711,12 @@
         <v>0</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>1701</v>
@@ -3732,12 +3726,12 @@
         <v>0</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>1801</v>
@@ -3747,12 +3741,12 @@
         <v>0</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>1802</v>
@@ -3762,12 +3756,12 @@
         <v>0</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>1803</v>
@@ -3777,12 +3771,12 @@
         <v>0</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>1901</v>
@@ -3792,12 +3786,12 @@
         <v>0</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>1803</v>
@@ -3807,12 +3801,12 @@
         <v>0</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>2101</v>
@@ -3822,12 +3816,12 @@
         <v>0</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>2201</v>
@@ -3837,12 +3831,12 @@
         <v>0</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>2301</v>
@@ -3852,12 +3846,12 @@
         <v>0</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>1</v>
@@ -3867,12 +3861,12 @@
         <v>0</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>2</v>
@@ -3882,12 +3876,12 @@
         <v>0</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>3</v>
@@ -3897,12 +3891,12 @@
         <v>0</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>1</v>
@@ -3912,12 +3906,12 @@
         <v>0</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>2</v>
@@ -3927,12 +3921,12 @@
         <v>0</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>3</v>
@@ -3942,12 +3936,12 @@
         <v>0</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>4</v>
@@ -3957,12 +3951,12 @@
         <v>0</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>5</v>
@@ -3972,12 +3966,12 @@
         <v>0</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>1</v>
@@ -3987,12 +3981,12 @@
         <v>0</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>2</v>
@@ -4002,12 +3996,12 @@
         <v>0</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>3</v>
@@ -4017,12 +4011,12 @@
         <v>0</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>4</v>
@@ -4032,12 +4026,12 @@
         <v>0</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>5</v>
@@ -4047,12 +4041,12 @@
         <v>0</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>6</v>
@@ -4062,12 +4056,12 @@
         <v>0</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>1</v>
@@ -4077,12 +4071,12 @@
         <v>0</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>2</v>
@@ -4092,12 +4086,12 @@
         <v>0</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>3</v>
@@ -4107,12 +4101,12 @@
         <v>0</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>4</v>
@@ -4122,12 +4116,12 @@
         <v>0</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>5</v>
@@ -4137,12 +4131,12 @@
         <v>0</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>6</v>
@@ -4152,12 +4146,12 @@
         <v>0</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>0</v>
@@ -4167,12 +4161,12 @@
         <v>0</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>1</v>
@@ -4182,7 +4176,7 @@
         <v>0</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed valueType categorical from trimester_rep
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_0/1_0_trimester_rep.xlsx
+++ b/dictionaries/urban_ath/1_0/1_0_trimester_rep.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26412"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_C32B3D6CD91DDAEC06AAB3A1401B85503AF5EB9E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37B5FC4C-0BCF-4F72-85CA-BB3BC5C9AADD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D26A6440-B6BF-4CF3-A116-40BFB2586FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="302">
   <si>
     <t>name</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>urb_area_id</t>
-  </si>
-  <si>
-    <t>categorical</t>
   </si>
   <si>
     <t>unique identifier for the urban area</t>
@@ -1765,7 +1762,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
   <cols>
@@ -1842,1327 +1841,1327 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
         <v>40</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
         <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
         <v>48</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
         <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
         <v>56</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
         <v>58</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
         <v>60</v>
-      </c>
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
         <v>62</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
         <v>66</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" t="s">
         <v>68</v>
-      </c>
-      <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>71</v>
-      </c>
-      <c r="D31" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+      <c r="D32" t="s">
         <v>73</v>
-      </c>
-      <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
         <v>75</v>
       </c>
-      <c r="B33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>76</v>
-      </c>
-      <c r="D33" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" t="s">
         <v>78</v>
-      </c>
-      <c r="B34" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-      <c r="D34" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
         <v>80</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>81</v>
-      </c>
-      <c r="D35" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
         <v>83</v>
-      </c>
-      <c r="B36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" t="s">
         <v>85</v>
       </c>
-      <c r="B37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>86</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" t="s">
         <v>88</v>
-      </c>
-      <c r="B38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
         <v>90</v>
-      </c>
-      <c r="B39" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" t="s">
-        <v>86</v>
-      </c>
-      <c r="D39" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" t="s">
         <v>92</v>
-      </c>
-      <c r="B40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" t="s">
         <v>94</v>
-      </c>
-      <c r="B41" t="s">
-        <v>19</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+      <c r="D42" t="s">
         <v>96</v>
-      </c>
-      <c r="B42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" t="s">
-        <v>86</v>
-      </c>
-      <c r="D42" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
         <v>98</v>
       </c>
-      <c r="B43" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>99</v>
-      </c>
-      <c r="D43" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
         <v>101</v>
-      </c>
-      <c r="B44" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
         <v>103</v>
-      </c>
-      <c r="B45" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
-        <v>99</v>
-      </c>
-      <c r="D45" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" t="s">
         <v>105</v>
       </c>
-      <c r="B46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>106</v>
-      </c>
-      <c r="D46" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>109</v>
-      </c>
-      <c r="D47" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48" t="s">
+        <v>108</v>
+      </c>
+      <c r="D48" t="s">
         <v>111</v>
-      </c>
-      <c r="B48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C48" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49" t="s">
         <v>113</v>
       </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>114</v>
-      </c>
-      <c r="D49" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>115</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50" t="s">
         <v>116</v>
-      </c>
-      <c r="B50" t="s">
-        <v>19</v>
-      </c>
-      <c r="C50" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
         <v>118</v>
       </c>
-      <c r="B51" t="s">
-        <v>19</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>119</v>
-      </c>
-      <c r="D51" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D52" t="s">
         <v>121</v>
-      </c>
-      <c r="B52" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" t="s">
-        <v>119</v>
-      </c>
-      <c r="D52" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" t="s">
+        <v>118</v>
+      </c>
+      <c r="D53" t="s">
         <v>123</v>
-      </c>
-      <c r="B53" t="s">
-        <v>19</v>
-      </c>
-      <c r="C53" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" t="s">
         <v>125</v>
-      </c>
-      <c r="B54" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" t="s">
-        <v>114</v>
-      </c>
-      <c r="D54" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
+        <v>126</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" t="s">
+        <v>113</v>
+      </c>
+      <c r="D55" t="s">
         <v>127</v>
-      </c>
-      <c r="B55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
         <v>129</v>
-      </c>
-      <c r="B56" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" t="s">
-        <v>114</v>
-      </c>
-      <c r="D56" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
+        <v>130</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" t="s">
         <v>131</v>
-      </c>
-      <c r="B57" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" t="s">
-        <v>114</v>
-      </c>
-      <c r="D57" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
+        <v>132</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
         <v>133</v>
-      </c>
-      <c r="B58" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
         <v>135</v>
-      </c>
-      <c r="B59" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
+        <v>136</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
         <v>137</v>
-      </c>
-      <c r="B60" t="s">
-        <v>19</v>
-      </c>
-      <c r="D60" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
+        <v>138</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" t="s">
         <v>139</v>
-      </c>
-      <c r="B61" t="s">
-        <v>19</v>
-      </c>
-      <c r="C61" t="s">
-        <v>99</v>
-      </c>
-      <c r="D61" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" t="s">
         <v>141</v>
-      </c>
-      <c r="B62" t="s">
-        <v>19</v>
-      </c>
-      <c r="C62" t="s">
-        <v>99</v>
-      </c>
-      <c r="D62" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
+        <v>142</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" t="s">
         <v>143</v>
-      </c>
-      <c r="B63" t="s">
-        <v>19</v>
-      </c>
-      <c r="C63" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" t="s">
         <v>145</v>
-      </c>
-      <c r="B64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C64" t="s">
-        <v>99</v>
-      </c>
-      <c r="D64" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
+        <v>146</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" t="s">
         <v>147</v>
-      </c>
-      <c r="B65" t="s">
-        <v>19</v>
-      </c>
-      <c r="C65" t="s">
-        <v>99</v>
-      </c>
-      <c r="D65" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
+        <v>148</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" t="s">
         <v>149</v>
-      </c>
-      <c r="B66" t="s">
-        <v>19</v>
-      </c>
-      <c r="C66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D66" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" t="s">
         <v>151</v>
-      </c>
-      <c r="B67" t="s">
-        <v>19</v>
-      </c>
-      <c r="C67" t="s">
-        <v>99</v>
-      </c>
-      <c r="D67" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" t="s">
         <v>153</v>
-      </c>
-      <c r="B68" t="s">
-        <v>19</v>
-      </c>
-      <c r="C68" t="s">
-        <v>99</v>
-      </c>
-      <c r="D68" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>98</v>
+      </c>
+      <c r="D69" t="s">
         <v>155</v>
-      </c>
-      <c r="B69" t="s">
-        <v>19</v>
-      </c>
-      <c r="C69" t="s">
-        <v>99</v>
-      </c>
-      <c r="D69" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
+        <v>156</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" t="s">
         <v>157</v>
-      </c>
-      <c r="B70" t="s">
-        <v>19</v>
-      </c>
-      <c r="C70" t="s">
-        <v>99</v>
-      </c>
-      <c r="D70" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
+        <v>158</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" t="s">
         <v>159</v>
-      </c>
-      <c r="B71" t="s">
-        <v>19</v>
-      </c>
-      <c r="C71" t="s">
-        <v>99</v>
-      </c>
-      <c r="D71" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
+        <v>160</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72" t="s">
+        <v>98</v>
+      </c>
+      <c r="D72" t="s">
         <v>161</v>
-      </c>
-      <c r="B72" t="s">
-        <v>19</v>
-      </c>
-      <c r="C72" t="s">
-        <v>99</v>
-      </c>
-      <c r="D72" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
       </c>
       <c r="D73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
       </c>
       <c r="D74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75" t="s">
         <v>167</v>
       </c>
-      <c r="B75" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>168</v>
-      </c>
-      <c r="D75" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
+        <v>169</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76" t="s">
         <v>170</v>
       </c>
-      <c r="B76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>171</v>
-      </c>
-      <c r="D76" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
+        <v>172</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77" t="s">
+        <v>170</v>
+      </c>
+      <c r="D77" t="s">
         <v>173</v>
-      </c>
-      <c r="B77" t="s">
-        <v>19</v>
-      </c>
-      <c r="C77" t="s">
-        <v>171</v>
-      </c>
-      <c r="D77" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
+        <v>174</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78" t="s">
         <v>175</v>
       </c>
-      <c r="B78" t="s">
-        <v>19</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>176</v>
-      </c>
-      <c r="D78" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
+        <v>177</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" t="s">
         <v>178</v>
       </c>
-      <c r="B79" t="s">
-        <v>19</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>179</v>
-      </c>
-      <c r="D79" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
+        <v>180</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80" t="s">
+        <v>178</v>
+      </c>
+      <c r="D80" t="s">
         <v>181</v>
-      </c>
-      <c r="B80" t="s">
-        <v>19</v>
-      </c>
-      <c r="C80" t="s">
-        <v>179</v>
-      </c>
-      <c r="D80" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
       </c>
       <c r="D82" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
+        <v>186</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" t="s">
         <v>187</v>
-      </c>
-      <c r="B83" t="s">
-        <v>19</v>
-      </c>
-      <c r="C83" t="s">
-        <v>71</v>
-      </c>
-      <c r="D83" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
+        <v>188</v>
+      </c>
+      <c r="B84" t="s">
+        <v>18</v>
+      </c>
+      <c r="C84" t="s">
+        <v>113</v>
+      </c>
+      <c r="D84" t="s">
         <v>189</v>
-      </c>
-      <c r="B84" t="s">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s">
-        <v>114</v>
-      </c>
-      <c r="D84" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
+        <v>190</v>
+      </c>
+      <c r="B85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" t="s">
         <v>191</v>
       </c>
-      <c r="B85" t="s">
-        <v>19</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>192</v>
-      </c>
-      <c r="D85" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
+        <v>193</v>
+      </c>
+      <c r="B86" t="s">
+        <v>18</v>
+      </c>
+      <c r="C86" t="s">
+        <v>191</v>
+      </c>
+      <c r="D86" t="s">
         <v>194</v>
-      </c>
-      <c r="B86" t="s">
-        <v>19</v>
-      </c>
-      <c r="C86" t="s">
-        <v>192</v>
-      </c>
-      <c r="D86" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
+        <v>195</v>
+      </c>
+      <c r="B87" t="s">
+        <v>18</v>
+      </c>
+      <c r="C87" t="s">
+        <v>191</v>
+      </c>
+      <c r="D87" t="s">
         <v>196</v>
-      </c>
-      <c r="B87" t="s">
-        <v>19</v>
-      </c>
-      <c r="C87" t="s">
-        <v>192</v>
-      </c>
-      <c r="D87" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
+        <v>197</v>
+      </c>
+      <c r="B88" t="s">
+        <v>18</v>
+      </c>
+      <c r="C88" t="s">
+        <v>98</v>
+      </c>
+      <c r="D88" t="s">
         <v>198</v>
-      </c>
-      <c r="B88" t="s">
-        <v>19</v>
-      </c>
-      <c r="C88" t="s">
-        <v>99</v>
-      </c>
-      <c r="D88" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
+        <v>199</v>
+      </c>
+      <c r="B89" t="s">
+        <v>18</v>
+      </c>
+      <c r="C89" t="s">
+        <v>98</v>
+      </c>
+      <c r="D89" t="s">
         <v>200</v>
-      </c>
-      <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" t="s">
-        <v>99</v>
-      </c>
-      <c r="D89" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
+        <v>201</v>
+      </c>
+      <c r="B90" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" t="s">
+        <v>98</v>
+      </c>
+      <c r="D90" t="s">
         <v>202</v>
-      </c>
-      <c r="B90" t="s">
-        <v>19</v>
-      </c>
-      <c r="C90" t="s">
-        <v>99</v>
-      </c>
-      <c r="D90" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
+        <v>203</v>
+      </c>
+      <c r="B91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C91" t="s">
+        <v>191</v>
+      </c>
+      <c r="D91" t="s">
         <v>204</v>
-      </c>
-      <c r="B91" t="s">
-        <v>19</v>
-      </c>
-      <c r="C91" t="s">
-        <v>192</v>
-      </c>
-      <c r="D91" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
+        <v>205</v>
+      </c>
+      <c r="B92" t="s">
+        <v>18</v>
+      </c>
+      <c r="C92" t="s">
+        <v>191</v>
+      </c>
+      <c r="D92" t="s">
         <v>206</v>
-      </c>
-      <c r="B92" t="s">
-        <v>19</v>
-      </c>
-      <c r="C92" t="s">
-        <v>192</v>
-      </c>
-      <c r="D92" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
+        <v>207</v>
+      </c>
+      <c r="B93" t="s">
+        <v>18</v>
+      </c>
+      <c r="C93" t="s">
+        <v>191</v>
+      </c>
+      <c r="D93" t="s">
         <v>208</v>
-      </c>
-      <c r="B93" t="s">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s">
-        <v>192</v>
-      </c>
-      <c r="D93" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
+        <v>209</v>
+      </c>
+      <c r="B94" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" t="s">
+        <v>98</v>
+      </c>
+      <c r="D94" t="s">
         <v>210</v>
-      </c>
-      <c r="B94" t="s">
-        <v>19</v>
-      </c>
-      <c r="C94" t="s">
-        <v>99</v>
-      </c>
-      <c r="D94" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
+        <v>211</v>
+      </c>
+      <c r="B95" t="s">
+        <v>18</v>
+      </c>
+      <c r="C95" t="s">
         <v>212</v>
       </c>
-      <c r="B95" t="s">
-        <v>19</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>213</v>
-      </c>
-      <c r="D95" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
+        <v>214</v>
+      </c>
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" t="s">
         <v>215</v>
       </c>
-      <c r="B96" t="s">
-        <v>19</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>216</v>
-      </c>
-      <c r="D96" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
+        <v>217</v>
+      </c>
+      <c r="B97" t="s">
+        <v>18</v>
+      </c>
+      <c r="C97" t="s">
         <v>218</v>
       </c>
-      <c r="B97" t="s">
-        <v>19</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
         <v>219</v>
-      </c>
-      <c r="D97" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
+        <v>220</v>
+      </c>
+      <c r="B98" t="s">
+        <v>18</v>
+      </c>
+      <c r="C98" t="s">
         <v>221</v>
       </c>
-      <c r="B98" t="s">
-        <v>19</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>222</v>
-      </c>
-      <c r="D98" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
+        <v>223</v>
+      </c>
+      <c r="B99" t="s">
+        <v>18</v>
+      </c>
+      <c r="C99" t="s">
+        <v>221</v>
+      </c>
+      <c r="D99" t="s">
         <v>224</v>
-      </c>
-      <c r="B99" t="s">
-        <v>19</v>
-      </c>
-      <c r="C99" t="s">
-        <v>222</v>
-      </c>
-      <c r="D99" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
+        <v>225</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" t="s">
+        <v>221</v>
+      </c>
+      <c r="D100" t="s">
         <v>226</v>
-      </c>
-      <c r="B100" t="s">
-        <v>19</v>
-      </c>
-      <c r="C100" t="s">
-        <v>222</v>
-      </c>
-      <c r="D100" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
+        <v>227</v>
+      </c>
+      <c r="B101" t="s">
+        <v>18</v>
+      </c>
+      <c r="C101" t="s">
+        <v>191</v>
+      </c>
+      <c r="D101" t="s">
         <v>228</v>
-      </c>
-      <c r="B101" t="s">
-        <v>19</v>
-      </c>
-      <c r="C101" t="s">
-        <v>192</v>
-      </c>
-      <c r="D101" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
+        <v>229</v>
+      </c>
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" t="s">
+        <v>70</v>
+      </c>
+      <c r="D102" t="s">
         <v>230</v>
-      </c>
-      <c r="B102" t="s">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s">
-        <v>71</v>
-      </c>
-      <c r="D102" t="s">
-        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -3188,13 +3187,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>232</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>233</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -3202,7 +3201,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B2">
         <v>101</v>
@@ -3211,12 +3210,12 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3">
         <v>102</v>
@@ -3225,12 +3224,12 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4">
         <v>103</v>
@@ -3239,12 +3238,12 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5">
         <v>104</v>
@@ -3253,12 +3252,12 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6">
         <v>105</v>
@@ -3267,12 +3266,12 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B7">
         <v>106</v>
@@ -3281,12 +3280,12 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8">
         <v>107</v>
@@ -3295,12 +3294,12 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9">
         <v>108</v>
@@ -3309,12 +3308,12 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10">
         <v>109</v>
@@ -3323,12 +3322,12 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11">
         <v>110</v>
@@ -3337,12 +3336,12 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12">
         <v>111</v>
@@ -3351,12 +3350,12 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B13">
         <v>112</v>
@@ -3365,12 +3364,12 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B14">
         <v>113</v>
@@ -3379,12 +3378,12 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B15">
         <v>114</v>
@@ -3393,12 +3392,12 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B16">
         <v>115</v>
@@ -3407,12 +3406,12 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17">
         <v>116</v>
@@ -3421,12 +3420,12 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B18">
         <v>117</v>
@@ -3435,12 +3434,12 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B19">
         <v>118</v>
@@ -3449,12 +3448,12 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B20">
         <v>119</v>
@@ -3463,12 +3462,12 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B21">
         <v>120</v>
@@ -3477,12 +3476,12 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B22">
         <v>121</v>
@@ -3491,12 +3490,12 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B23">
         <v>122</v>
@@ -3505,12 +3504,12 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B24">
         <v>123</v>
@@ -3519,12 +3518,12 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B25">
         <v>124</v>
@@ -3533,12 +3532,12 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B26">
         <v>125</v>
@@ -3547,12 +3546,12 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B27">
         <v>126</v>
@@ -3561,12 +3560,12 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28">
         <v>127</v>
@@ -3575,12 +3574,12 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29">
         <v>128</v>
@@ -3589,12 +3588,12 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B30">
         <v>129</v>
@@ -3603,12 +3602,12 @@
         <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B31">
         <v>130</v>
@@ -3617,12 +3616,12 @@
         <v>0</v>
       </c>
       <c r="D31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B32">
         <v>131</v>
@@ -3631,7 +3630,7 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -3645,7 +3644,7 @@
         <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -3659,7 +3658,7 @@
         <v>0</v>
       </c>
       <c r="D34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -3673,7 +3672,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -3687,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -3701,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -3715,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -3729,7 +3728,7 @@
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -3743,7 +3742,7 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -3757,7 +3756,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -3771,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -3785,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -3799,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -3813,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -3827,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -3841,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="D47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3855,7 +3854,7 @@
         <v>0</v>
       </c>
       <c r="D48" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -3869,7 +3868,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -3883,7 +3882,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -3897,7 +3896,7 @@
         <v>0</v>
       </c>
       <c r="D51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3911,7 +3910,7 @@
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -3925,7 +3924,7 @@
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3939,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3953,7 +3952,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -3967,7 +3966,7 @@
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -3981,12 +3980,12 @@
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -3995,12 +3994,12 @@
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B59">
         <v>2</v>
@@ -4009,12 +4008,12 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B60">
         <v>3</v>
@@ -4023,12 +4022,12 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -4037,12 +4036,12 @@
         <v>0</v>
       </c>
       <c r="D61" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B62">
         <v>2</v>
@@ -4051,12 +4050,12 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B63">
         <v>3</v>
@@ -4065,12 +4064,12 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B64">
         <v>4</v>
@@ -4079,12 +4078,12 @@
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B65">
         <v>5</v>
@@ -4093,12 +4092,12 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -4107,12 +4106,12 @@
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B67">
         <v>2</v>
@@ -4121,12 +4120,12 @@
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B68">
         <v>3</v>
@@ -4135,12 +4134,12 @@
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B69">
         <v>4</v>
@@ -4149,12 +4148,12 @@
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -4163,12 +4162,12 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B71">
         <v>6</v>
@@ -4177,12 +4176,12 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -4191,12 +4190,12 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -4205,12 +4204,12 @@
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B74">
         <v>3</v>
@@ -4219,12 +4218,12 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B75">
         <v>4</v>
@@ -4233,12 +4232,12 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B76">
         <v>5</v>
@@ -4247,12 +4246,12 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B77">
         <v>6</v>
@@ -4261,12 +4260,12 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -4275,12 +4274,12 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -4289,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>